<commit_message>
Added EMO2019. Shifted some things.
</commit_message>
<xml_diff>
--- a/notable-conferences.xlsx
+++ b/notable-conferences.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AProjects\notable_conferences\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\notable-conferences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{20EB096A-1625-4332-9BF0-C6F24817EEA4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2153E2-7B0C-4E61-84B0-853C24F7CC8F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23220" windowHeight="10830" xr2:uid="{0A52E70F-C8F4-4670-AACD-D6FC6901FB02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -343,6 +343,18 @@
   </si>
   <si>
     <t>Every other year</t>
+  </si>
+  <si>
+    <t>Evolutionary Multi-Criterion Optimization</t>
+  </si>
+  <si>
+    <t>EMO</t>
+  </si>
+  <si>
+    <t>E. Lansing</t>
+  </si>
+  <si>
+    <t>MCDM</t>
   </si>
 </sst>
 </file>
@@ -720,34 +732,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE1C0D8-9679-4C85-BD45-EEBF7903559E}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -794,7 +806,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -838,70 +850,38 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>43240</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>43244</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2018</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="4">
-        <v>43275</v>
-      </c>
-      <c r="D6" s="4">
-        <v>43279</v>
       </c>
       <c r="E6" s="3">
         <v>2018</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" t="s">
@@ -912,33 +892,33 @@
       </c>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4">
-        <v>43317</v>
+        <v>43275</v>
       </c>
       <c r="D7" s="4">
-        <v>43322</v>
+        <v>43279</v>
       </c>
       <c r="E7" s="3">
         <v>2018</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>46</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" t="s">
@@ -949,33 +929,33 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4">
-        <v>43331</v>
+        <v>43317</v>
       </c>
       <c r="D8" s="4">
-        <v>43335</v>
+        <v>43322</v>
       </c>
       <c r="E8" s="3">
         <v>2018</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>46</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" t="s">
@@ -986,33 +966,33 @@
       </c>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4">
-        <v>43408</v>
+        <v>43331</v>
       </c>
       <c r="D9" s="4">
-        <v>43412</v>
+        <v>43335</v>
       </c>
       <c r="E9" s="3">
         <v>2018</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>46</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" t="s">
@@ -1022,73 +1002,74 @@
         <v>72</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" t="s">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="4">
+        <v>43408</v>
+      </c>
+      <c r="D10" s="4">
+        <v>43412</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2018</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>43408</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>43413</v>
-      </c>
-      <c r="E10" s="2">
-        <v>2018</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K10" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1">
-        <v>43437</v>
-      </c>
-      <c r="D11" s="1">
-        <v>43441</v>
       </c>
       <c r="E11" s="2">
         <v>2018</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" t="s">
         <v>46</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
         <v>72</v>
@@ -1098,18 +1079,18 @@
       </c>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>43444</v>
+        <v>43437</v>
       </c>
       <c r="D12" s="1">
-        <v>43448</v>
+        <v>43441</v>
       </c>
       <c r="E12" s="2">
         <v>2018</v>
@@ -1124,10 +1105,7 @@
         <v>46</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="5">
-        <v>25000</v>
+        <v>45</v>
       </c>
       <c r="K12" t="s">
         <v>72</v>
@@ -1137,33 +1115,36 @@
       </c>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1">
-        <v>43442</v>
+        <v>43444</v>
       </c>
       <c r="D13" s="1">
-        <v>43447</v>
+        <v>43448</v>
       </c>
       <c r="E13" s="2">
         <v>2018</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H13" t="s">
         <v>46</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="J13" s="5">
+        <v>25000</v>
       </c>
       <c r="K13" t="s">
         <v>72</v>
@@ -1173,71 +1154,69 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
-        <v>43296</v>
+        <v>43442</v>
       </c>
       <c r="D14" s="1">
-        <v>43300</v>
+        <v>43447</v>
       </c>
       <c r="E14" s="2">
         <v>2018</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" t="s">
-        <v>99</v>
+        <v>46</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="K14" t="s">
         <v>72</v>
       </c>
-      <c r="L14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1">
-        <v>43408</v>
+        <v>43296</v>
       </c>
       <c r="D15" s="1">
-        <v>43411</v>
+        <v>43300</v>
       </c>
       <c r="E15" s="2">
         <v>2018</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I15" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" s="5">
-        <v>5000</v>
+        <v>99</v>
       </c>
       <c r="K15" t="s">
         <v>72</v>
@@ -1246,339 +1225,407 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="1">
-        <v>43276</v>
+        <v>43408</v>
       </c>
       <c r="D16" s="1">
-        <v>43280</v>
+        <v>43411</v>
       </c>
       <c r="E16" s="2">
         <v>2018</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H16" t="s">
         <v>86</v>
       </c>
       <c r="I16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="5">
+        <v>5000</v>
+      </c>
+      <c r="K16" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43276</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43280</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" t="s">
         <v>89</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J17" s="5">
         <v>1500</v>
       </c>
-      <c r="K16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="1">
-        <v>43184</v>
-      </c>
-      <c r="D18" s="1">
-        <v>43188</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2019</v>
-      </c>
-      <c r="F18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" t="s">
-        <v>72</v>
-      </c>
-      <c r="L18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="C19" s="1">
-        <v>43239</v>
+        <v>43169</v>
       </c>
       <c r="D19" s="1">
-        <v>43243</v>
+        <v>43172</v>
       </c>
       <c r="E19" s="2">
         <v>2019</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H19" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K19" t="s">
-        <v>72</v>
-      </c>
-      <c r="L19" s="7">
-        <v>43136</v>
-      </c>
-      <c r="M19" s="7"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1">
-        <v>43261</v>
+        <v>43184</v>
       </c>
       <c r="D20" s="1">
-        <v>43265</v>
+        <v>43188</v>
       </c>
       <c r="E20" s="2">
         <v>2019</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H20" t="s">
         <v>46</v>
       </c>
       <c r="I20" t="s">
-        <v>47</v>
-      </c>
-      <c r="K20" s="7">
-        <v>43425</v>
-      </c>
-      <c r="N20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="K20" t="s">
+        <v>72</v>
+      </c>
+      <c r="L20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1">
-        <v>43323</v>
+        <v>43239</v>
       </c>
       <c r="D21" s="1">
-        <v>43328</v>
+        <v>43243</v>
       </c>
       <c r="E21" s="2">
         <v>2019</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H21" t="s">
         <v>46</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K21" s="7">
-        <v>43419</v>
-      </c>
-      <c r="N21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K21" t="s">
+        <v>72</v>
+      </c>
+      <c r="L21" s="7">
+        <v>43136</v>
+      </c>
+      <c r="M21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1">
-        <v>43407</v>
+        <v>43261</v>
       </c>
       <c r="D22" s="1">
-        <v>43411</v>
+        <v>43264</v>
       </c>
       <c r="E22" s="2">
         <v>2019</v>
       </c>
       <c r="F22" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="G22" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="I22" t="s">
-        <v>69</v>
-      </c>
-      <c r="N22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1">
-        <v>43407</v>
+        <v>43261</v>
       </c>
       <c r="D23" s="1">
-        <v>43411</v>
+        <v>43265</v>
       </c>
       <c r="E23" s="2">
         <v>2019</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H23" t="s">
         <v>46</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="K23" s="7">
+        <v>43425</v>
+      </c>
+      <c r="N23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1">
-        <v>43443</v>
+        <v>43323</v>
       </c>
       <c r="D24" s="1">
-        <v>43447</v>
+        <v>43328</v>
       </c>
       <c r="E24" s="2">
         <v>2019</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H24" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="I24" t="s">
-        <v>66</v>
-      </c>
-      <c r="J24" s="5">
-        <v>25000</v>
-      </c>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="K24" s="7">
+        <v>43419</v>
+      </c>
+      <c r="N24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43407</v>
+      </c>
+      <c r="D25" s="1">
+        <v>43411</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" t="s">
+        <v>69</v>
+      </c>
+      <c r="N25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1">
-        <v>43261</v>
+        <v>43407</v>
       </c>
       <c r="D26" s="1">
-        <v>43264</v>
+        <v>43411</v>
       </c>
       <c r="E26" s="2">
         <v>2019</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="I26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43443</v>
+      </c>
+      <c r="D27" s="1">
+        <v>43447</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="5">
+        <v>25000</v>
+      </c>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Salmon Recovery Conference 2019
</commit_message>
<xml_diff>
--- a/notable-conferences.xlsx
+++ b/notable-conferences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitProjects\notable-conferences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{316EDF69-BD17-4316-8FFD-AD473119AD46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{98C8B6D7-3FAA-4E7B-BB1F-094B96F69CA5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23220" windowHeight="10830" xr2:uid="{0A52E70F-C8F4-4670-AACD-D6FC6901FB02}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="137">
   <si>
     <t>Name</t>
   </si>
@@ -421,6 +421,21 @@
   </si>
   <si>
     <t>Pulping</t>
+  </si>
+  <si>
+    <t>Salmon Recoverry Conference</t>
+  </si>
+  <si>
+    <t>Tacoma</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Puget Sound</t>
+  </si>
+  <si>
+    <t>https://www.rco.wa.gov/salmon_recovery/2019-SalmonConference/Confhome.shtml</t>
   </si>
 </sst>
 </file>
@@ -799,11 +814,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE1C0D8-9679-4C85-BD45-EEBF7903559E}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,187 +1528,187 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C23" s="1">
-        <v>43239</v>
+        <v>43198</v>
       </c>
       <c r="D23" s="1">
-        <v>43243</v>
+        <v>43199</v>
       </c>
       <c r="E23" s="2">
         <v>2019</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>134</v>
       </c>
       <c r="H23" t="s">
         <v>45</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
-      </c>
-      <c r="K23" t="s">
-        <v>71</v>
-      </c>
-      <c r="L23" s="7">
-        <v>43136</v>
-      </c>
-      <c r="M23" s="7"/>
+        <v>135</v>
+      </c>
+      <c r="J23">
+        <v>800</v>
+      </c>
+      <c r="N23" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1">
-        <v>43261</v>
+        <v>43239</v>
       </c>
       <c r="D24" s="1">
-        <v>43264</v>
+        <v>43243</v>
       </c>
       <c r="E24" s="2">
         <v>2019</v>
       </c>
       <c r="F24" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="H24" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="I24" t="s">
-        <v>87</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="K24" t="s">
+        <v>71</v>
+      </c>
+      <c r="L24" s="7">
+        <v>43136</v>
+      </c>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C25" s="1">
         <v>43261</v>
       </c>
       <c r="D25" s="1">
-        <v>43265</v>
+        <v>43264</v>
       </c>
       <c r="E25" s="2">
         <v>2019</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="G25" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="H25" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s">
-        <v>46</v>
-      </c>
-      <c r="K25" s="7">
-        <v>43425</v>
-      </c>
-      <c r="N25" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="C26" s="1">
-        <v>43294</v>
+        <v>43261</v>
       </c>
       <c r="D26" s="1">
-        <v>43298</v>
+        <v>43265</v>
       </c>
       <c r="E26" s="2">
         <v>2019</v>
       </c>
       <c r="F26" t="s">
-        <v>123</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="I26" t="s">
-        <v>97</v>
-      </c>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7">
-        <v>43495</v>
-      </c>
-      <c r="N26" s="10" t="s">
-        <v>125</v>
+        <v>46</v>
+      </c>
+      <c r="K26" s="7">
+        <v>43425</v>
+      </c>
+      <c r="N26" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C27" s="1">
-        <v>43323</v>
+        <v>43294</v>
       </c>
       <c r="D27" s="1">
-        <v>43328</v>
+        <v>43298</v>
       </c>
       <c r="E27" s="2">
         <v>2019</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="G27" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="I27" t="s">
-        <v>61</v>
-      </c>
-      <c r="K27" s="7">
-        <v>43419</v>
-      </c>
-      <c r="N27" t="s">
-        <v>77</v>
+        <v>97</v>
+      </c>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7">
+        <v>43495</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="C28" s="1">
-        <v>43403</v>
+        <v>43323</v>
       </c>
       <c r="D28" s="1">
-        <v>43407</v>
+        <v>43328</v>
       </c>
       <c r="E28" s="2">
         <v>2019</v>
@@ -1708,48 +1723,51 @@
         <v>45</v>
       </c>
       <c r="I28" t="s">
-        <v>112</v>
-      </c>
-      <c r="K28" s="7"/>
+        <v>61</v>
+      </c>
+      <c r="K28" s="7">
+        <v>43419</v>
+      </c>
+      <c r="N28" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="C29" s="1">
+        <v>43403</v>
+      </c>
+      <c r="D29" s="1">
         <v>43407</v>
-      </c>
-      <c r="D29" s="1">
-        <v>43411</v>
       </c>
       <c r="E29" s="2">
         <v>2019</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H29" t="s">
         <v>45</v>
       </c>
       <c r="I29" t="s">
-        <v>68</v>
-      </c>
-      <c r="N29" t="s">
-        <v>76</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1">
         <v>43407</v>
@@ -1761,129 +1779,161 @@
         <v>2019</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G30" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H30" t="s">
         <v>45</v>
       </c>
       <c r="I30" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="N30" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1">
-        <v>43435</v>
+        <v>43407</v>
       </c>
       <c r="D31" s="1">
-        <v>43440</v>
+        <v>43411</v>
       </c>
       <c r="E31" s="2">
         <v>2019</v>
       </c>
       <c r="F31" t="s">
-        <v>118</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
+        <v>31</v>
       </c>
       <c r="H31" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="I31" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31">
-        <v>900</v>
-      </c>
-      <c r="K31" s="7">
-        <v>43490</v>
-      </c>
-      <c r="L31" s="7">
-        <v>43677</v>
-      </c>
-      <c r="M31" s="7">
-        <v>43707</v>
-      </c>
-      <c r="N31" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="C32" s="1">
-        <v>43443</v>
+        <v>43435</v>
       </c>
       <c r="D32" s="1">
-        <v>43447</v>
+        <v>43440</v>
       </c>
       <c r="E32" s="2">
         <v>2019</v>
       </c>
       <c r="F32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32" t="s">
+        <v>119</v>
+      </c>
+      <c r="H32" t="s">
+        <v>59</v>
+      </c>
+      <c r="I32" t="s">
+        <v>61</v>
+      </c>
+      <c r="J32">
+        <v>900</v>
+      </c>
+      <c r="K32" s="7">
+        <v>43490</v>
+      </c>
+      <c r="L32" s="7">
+        <v>43677</v>
+      </c>
+      <c r="M32" s="7">
+        <v>43707</v>
+      </c>
+      <c r="N32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1">
+        <v>43443</v>
+      </c>
+      <c r="D33" s="1">
+        <v>43447</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F33" t="s">
         <v>69</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>25</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H33" t="s">
         <v>70</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I33" t="s">
         <v>65</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J33" s="5">
         <v>25000</v>
       </c>
-      <c r="K32" s="5"/>
-    </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="2"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-    </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
       <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>